<commit_message>
debug "put a big number",
Please enter the commit message for your changes. Lines starting
with '#' will be ignored, and an empty message aborts the commit.
On branch master
Changes to be committed:
	modified:   checkInput.txt
	modified:   inputData.xlsx
	new file:   inputpu.txt
	new file:   inputpu2.txt
	new file:   outpu.txt
	new file:   outpu2.txt
	new file:   outputpu2.txt
	modified:   src/trackFEA/Solver.java

Changes not staged for commit:
	deleted:    o2.txt
	deleted:    oo.txt
	deleted:    out50.txt

Untracked files:
	.classpath
	.gitignore
	.project
</commit_message>
<xml_diff>
--- a/inputData.xlsx
+++ b/inputData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79d2e06a4ad5c942/course/homework 2/fea program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DXX\OneDrive\course\homework 2\fea program\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="case1" sheetId="2" r:id="rId1"/>
-    <sheet name="origin" sheetId="1" r:id="rId2"/>
+    <sheet name="pu" sheetId="3" r:id="rId2"/>
+    <sheet name="pu2" sheetId="4" r:id="rId3"/>
+    <sheet name="origin" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
   <si>
     <t>analysisType: static or dynamics</t>
   </si>
@@ -486,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,10 +736,522 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <f>210000</f>
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="1">
+        <f>33000000</f>
+        <v>33000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <f>70/1000</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <f>9.82*10^6/10^6</f>
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1000</v>
+      </c>
+      <c r="G23">
+        <v>2000</v>
+      </c>
+      <c r="H23">
+        <v>3000</v>
+      </c>
+      <c r="I23">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <f>210000</f>
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="1">
+        <f>33000000</f>
+        <v>33000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <f>70/1000</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <f>9.82*10^6/10^6</f>
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1000</v>
+      </c>
+      <c r="G23">
+        <v>2000</v>
+      </c>
+      <c r="H23">
+        <v>3000</v>
+      </c>
+      <c r="I23">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A32"/>
   <sheetViews>

</xml_diff>